<commit_message>
change image size of Product page
</commit_message>
<xml_diff>
--- a/excel-data/Hats-data.xlsx
+++ b/excel-data/Hats-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bryan.joe.haboc\Desktop\Polder\the_odin_project\shop-app\excel-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67619E41-38F9-4912-AF36-5328E818B202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482A9B36-D01D-4433-8BD4-0EC7F81A1A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0076172B-D2D4-4D69-9279-9161EB17C274}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'output (1)'!$A$1:$D$10</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'output (1)'!$A$1:$E$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
   <si>
     <t>Brown Brim</t>
   </si>
@@ -115,16 +115,159 @@
   </si>
   <si>
     <t>Hats</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Brown Brim is a great way to add a little style to your face, so you can rock that funky, throwback style like Eminem!</t>
+  </si>
+  <si>
+    <t>Blue Beanie is a great color for this winter, a change from red and black. With a little bit of work, you can make it look even better.</t>
+  </si>
+  <si>
+    <t>This is a cowboy hat that is made of brown leather and has a three-point crown. The brim is notched and has brass tacks. It is in excellent condition and ready to sew up.</t>
+  </si>
+  <si>
+    <t>A Stylish, Affordable and Versatile Way to Get Cool, Comfortable Sun Protection</t>
+  </si>
+  <si>
+    <t>If you want beanie that stands out and looks great and keeps you warm, then these beanies are for you.</t>
+  </si>
+  <si>
+    <t>Add some immediate style to your wardrobe with this tropical palm tree cap. Any hat or cap can be made into a unique headwear statement, but for a budget-friendly look, this palm tree cap is the way to go.</t>
+  </si>
+  <si>
+    <t>This red beanie is a good way to start a conversation with a friend. It is a great gift for people who like a warm winter hat.</t>
+  </si>
+  <si>
+    <t>One of the most unique hats you will ever feel.</t>
+  </si>
+  <si>
+    <t>The most iconic cap of all time has a brand new look. The classic blue snapback hat has been given a subtle update.</t>
+  </si>
+  <si>
+    <t>https://images.pexels.com/photos/458649/pexels-photo-458649.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=2</t>
+  </si>
+  <si>
+    <t>White Sun Hat</t>
+  </si>
+  <si>
+    <t>A slightly slouchy and light-weight crochet sun hat for adults.</t>
+  </si>
+  <si>
+    <t>https://images.pexels.com/photos/984619/pexels-photo-984619.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=2</t>
+  </si>
+  <si>
+    <t>https://images.pexels.com/photos/235496/pexels-photo-235496.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=2</t>
+  </si>
+  <si>
+    <t>Pink Sun Hat</t>
+  </si>
+  <si>
+    <t>Brown Sun Hat</t>
+  </si>
+  <si>
+    <t>https://images.pexels.com/photos/33622/fashion-model-beach-hat.jpg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=2</t>
+  </si>
+  <si>
+    <t>Blue Sun Hat</t>
+  </si>
+  <si>
+    <t>https://images.pexels.com/photos/3651597/pexels-photo-3651597.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=2</t>
+  </si>
+  <si>
+    <t>Black Hat</t>
+  </si>
+  <si>
+    <t>https://images.pexels.com/photos/2453104/pexels-photo-2453104.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=2</t>
+  </si>
+  <si>
+    <t>Maroon Beanie</t>
+  </si>
+  <si>
+    <t>Blue Knitted Beanie</t>
+  </si>
+  <si>
+    <t>https://images.pexels.com/photos/2460527/pexels-photo-2460527.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=2</t>
+  </si>
+  <si>
+    <t>https://images.pexels.com/photos/2297362/pexels-photo-2297362.png?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=2</t>
+  </si>
+  <si>
+    <t>Black Cap</t>
+  </si>
+  <si>
+    <t>https://images.pexels.com/photos/3512491/pexels-photo-3512491.png?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=2</t>
+  </si>
+  <si>
+    <t>White Cap</t>
+  </si>
+  <si>
+    <t>https://images.pexels.com/photos/2092837/pexels-photo-2092837.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=2</t>
+  </si>
+  <si>
+    <t>Black Fedora</t>
+  </si>
+  <si>
+    <t>https://images.pexels.com/photos/3197314/pexels-photo-3197314.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> You can't go wrong with a woven hat. Made in the USA. </t>
+  </si>
+  <si>
+    <t>A funky pink sun hat that is the perfect accessory for your summer trips. The hat is made from a cotton and polyester blend, suitable for both men and women.</t>
+  </si>
+  <si>
+    <t>A funky blue sun hat that is the perfect accessory for your summer trips. The hat is made from a cotton and polyester blend, suitable for both men and women.</t>
+  </si>
+  <si>
+    <t>A funky black hat</t>
+  </si>
+  <si>
+    <t>This maroon beanie is a cool way to bring out the color of your outfit!</t>
+  </si>
+  <si>
+    <t>This pretty knitted beanie makes a great gift for any occasion. It's easy to make and you can choose from a variety of colours.</t>
+  </si>
+  <si>
+    <t>A black cap that is perfect for formal and semi-formal attire! Buy it now!</t>
+  </si>
+  <si>
+    <t>A white cap can be worn with just about anything, and it looks good with a suit, tie, or even with a t-shirt, polo, or sweater.</t>
+  </si>
+  <si>
+    <t>A black fedora is a classic accessory that can never go out of style. It's the perfect match for all of your fall outfits. Look great, feel great, and be seen!</t>
+  </si>
+  <si>
+    <t>Light Colored Sun Hat</t>
+  </si>
+  <si>
+    <t>A sun hat is a must-have accessory for the summer months. Many people don't realize that wearing a hat can protect your skin from the sun and help prevent sunburn. If you wear a hat, be sure to use one with a wide brim to help protect you from the sun.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -147,13 +290,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -171,10 +317,11 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{E328D36C-9457-4F73-B334-7EAB40649EED}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="5">
-    <queryTableFields count="4">
+  <queryTableRefresh nextId="6">
+    <queryTableFields count="5">
       <queryTableField id="1" name="Column1._id" tableColumnId="1"/>
       <queryTableField id="2" name="Column1.name" tableColumnId="2"/>
+      <queryTableField id="5" dataBound="0" tableColumnId="7"/>
       <queryTableField id="3" name="Column1.imageUrl" tableColumnId="3"/>
       <queryTableField id="4" name="Column1.price" tableColumnId="4"/>
     </queryTableFields>
@@ -183,11 +330,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5DFB531D-6892-42E3-A011-FB8172E18C60}" name="output__1" displayName="output__1" ref="A1:D10" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D10" xr:uid="{5DFB531D-6892-42E3-A011-FB8172E18C60}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5DFB531D-6892-42E3-A011-FB8172E18C60}" name="output__1" displayName="output__1" ref="A1:E21" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:E21" xr:uid="{5DFB531D-6892-42E3-A011-FB8172E18C60}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{67CF36C9-F95B-4D2B-8D5F-779A76A34C37}" uniqueName="1" name="title" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{54471A27-B057-41B2-BD91-97B503B1135A}" uniqueName="2" name="name" queryTableFieldId="2"/>
+    <tableColumn id="7" xr3:uid="{193928BD-2F8F-4086-80E5-F1CADB59CE5B}" uniqueName="7" name="description" queryTableFieldId="5"/>
     <tableColumn id="3" xr3:uid="{22B561C5-B055-462D-BAA2-92CC96BD423C}" uniqueName="3" name="imageUrl" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{A7C19A7B-4B46-451C-9736-34E0A18F7CC1}" uniqueName="4" name="price" queryTableFieldId="4"/>
   </tableColumns>
@@ -492,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB3E4F6-7FEE-4BC9-AFC2-D2C23D6BC02F}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -506,7 +654,7 @@
     <col min="4" max="4" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -514,13 +662,16 @@
         <v>19</v>
       </c>
       <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -528,13 +679,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -542,13 +696,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -556,13 +713,16 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -570,13 +730,16 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -584,13 +747,16 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -598,13 +764,16 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -612,13 +781,16 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -626,13 +798,16 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -640,17 +815,215 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
         <v>17</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>16</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D11" r:id="rId1" xr:uid="{122B866F-4A90-476B-A97B-9281E3597D56}"/>
+    <hyperlink ref="D12" r:id="rId2" xr:uid="{BE036483-7CB3-4D16-80AA-83FD9C159A7D}"/>
+    <hyperlink ref="D13" r:id="rId3" xr:uid="{4D1A8959-ED62-4C2B-848F-13807C7EA47E}"/>
+    <hyperlink ref="D18" r:id="rId4" xr:uid="{3F0F5249-145A-4D21-BEB7-F6D35321E52F}"/>
+    <hyperlink ref="D21" r:id="rId5" xr:uid="{8B24667C-E9C1-41AD-808C-581A3A80E642}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>